<commit_message>
Added the selection of collaborators for several projects
</commit_message>
<xml_diff>
--- a/employee_competence_table.xlsx
+++ b/employee_competence_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Роман\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Роман\PycharmProjects\Team_selection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ACD54EB-55D9-48CD-9DC6-2450A1B9051B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16FEEAF2-D827-4B14-89E4-DAC169E6FCFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16457" yWindow="0" windowWidth="16457" windowHeight="17914" xr2:uid="{866999C5-EB3E-4C00-90EB-A04A05C5DD20}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{866999C5-EB3E-4C00-90EB-A04A05C5DD20}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -455,7 +455,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>